<commit_message>
[CHG] ATUALIZANDO O MAPA DE STAKEHOLDERS
</commit_message>
<xml_diff>
--- a/Mapa de Stakeholders.xlsx
+++ b/Mapa de Stakeholders.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e66243f108409f2/Área de Trabalho/Itaú/CICF/Product Manager/excel-backlog-planning-roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="447" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9144CD0-7A9C-42E9-8D89-51181825ECDA}"/>
+  <xr:revisionPtr revIDLastSave="511" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{521ED50A-74A3-41BC-8A4F-A43640FE004E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entrevistados" sheetId="1" r:id="rId1"/>
-    <sheet name="Mapa de Stakeholders" sheetId="2" r:id="rId2"/>
-    <sheet name="Auxiliares" sheetId="3" r:id="rId3"/>
+    <sheet name="Comparativo Perfis Entrevistado" sheetId="4" r:id="rId2"/>
+    <sheet name="Mapa de Stakeholders" sheetId="2" r:id="rId3"/>
+    <sheet name="Auxiliares" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Lista_Comunicacao">INDIRECT("tbComunicacao[Comunicação Preferencial]")</definedName>
@@ -90,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="149">
   <si>
     <t>Grupo</t>
   </si>
@@ -447,9 +448,6 @@
     <t>Caio Eduardo Silva</t>
   </si>
   <si>
-    <t>Garantir eficiência e qualidade dos fornecedores de manutenção</t>
-  </si>
-  <si>
     <t>Análise de dispersão de SLA e Long tail, com causa raiz
 Informação de indisponibilidade por agência ofensoras
 Visualização por fornecedor</t>
@@ -488,13 +486,96 @@
   </si>
   <si>
     <t>Command Center</t>
+  </si>
+  <si>
+    <t>PM Produto</t>
+  </si>
+  <si>
+    <t>Liderança de Produto e Operação</t>
+  </si>
+  <si>
+    <t>Analista/Coord. de Operação</t>
+  </si>
+  <si>
+    <t>Foco</t>
+  </si>
+  <si>
+    <t>Execução e entrega de produto</t>
+  </si>
+  <si>
+    <t>Estratégia, performance e decisões macro</t>
+  </si>
+  <si>
+    <t>Frequência</t>
+  </si>
+  <si>
+    <t>Dados exigidos</t>
+  </si>
+  <si>
+    <t>Disponibilidade, saúde, alertas</t>
+  </si>
+  <si>
+    <t>Performance agregada, históricos, OKRs</t>
+  </si>
+  <si>
+    <t>SLA, reincidência, previsão, performance por fornecedor</t>
+  </si>
+  <si>
+    <t>Painel desejado</t>
+  </si>
+  <si>
+    <t>Interativo, com filtros</t>
+  </si>
+  <si>
+    <t>Analítico e consolidado</t>
+  </si>
+  <si>
+    <t>Tático e detalhado com filtros por fornecedor</t>
+  </si>
+  <si>
+    <t>Formato</t>
+  </si>
+  <si>
+    <t>Real time + histórico</t>
+  </si>
+  <si>
+    <t>Dispositivo</t>
+  </si>
+  <si>
+    <t>Eficiência e performance de fornecedores</t>
+  </si>
+  <si>
+    <t>Tomar decisões estratégicas com base em dados de disponibilidade de agência.</t>
+  </si>
+  <si>
+    <t>Garantir eficiência e qualidade dos fornecedores de manutenção.</t>
+  </si>
+  <si>
+    <t>Verificar se a agência está fechada de forma tempestiva
+Conseguir trocar pessoas entre agências com maior fluxo de clientes</t>
+  </si>
+  <si>
+    <t>Disponibilidade de agências
+Equipamentos inoperantes
+Quantidade de clientes na agência no momento</t>
+  </si>
+  <si>
+    <t>Visão de agências ou bairros indisponíveis
+Informação tempestiva para decisão
+SLA diferenciado conforme contexto da agência (ex: risco reputacional)</t>
+  </si>
+  <si>
+    <t>Fabiano Rezende Pellin</t>
+  </si>
+  <si>
+    <t>Rogerio Vasconcelos Costa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,6 +587,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -676,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -750,9 +839,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -768,9 +854,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -805,6 +888,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1314,10 +1406,10 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1382,30 +1474,30 @@
       <c r="D2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="J2" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="30" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B3" s="19" t="s">
@@ -1417,13 +1509,13 @@
       <c r="D3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="33"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="31"/>
     </row>
     <row r="4" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
@@ -1438,30 +1530,30 @@
       <c r="D4" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="J4" s="34" t="s">
+      <c r="J4" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="36" t="s">
+      <c r="K4" s="34" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="44" t="s">
         <v>66</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -1473,16 +1565,16 @@
       <c r="D5" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="37"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="35"/>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="25" t="s">
         <v>70</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -1494,13 +1586,13 @@
       <c r="D6" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="37"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="35"/>
     </row>
     <row r="7" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
@@ -1515,171 +1607,196 @@
       <c r="D7" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="37"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="35"/>
     </row>
     <row r="8" spans="1:11" ht="172.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="F8" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="G8" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="H8" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="I8" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="K8" s="40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+    </row>
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="27"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+    </row>
+    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+    </row>
+    <row r="12" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="G12" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="H12" s="43" t="s">
+        <v>146</v>
+      </c>
+      <c r="I12" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="42" t="s">
-        <v>116</v>
-      </c>
-      <c r="K8" s="42" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
-    </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-    </row>
-    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="30" t="s">
+      <c r="J12" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="K12" s="43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C13" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="30" t="s">
+      <c r="D13" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
+      <c r="D14" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="28">
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="I12:I14"/>
     <mergeCell ref="J8:J11"/>
     <mergeCell ref="K8:K11"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
     <mergeCell ref="E8:E11"/>
     <mergeCell ref="F8:F11"/>
     <mergeCell ref="G8:G11"/>
@@ -1705,6 +1822,122 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{896AFEEB-F632-4315-844F-C80E2D24D70E}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="4" width="29.88671875" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A74E9A74-8D70-4B21-BAA8-615D266582B4}">
   <dimension ref="A1:J23"/>
   <sheetViews>
@@ -2103,7 +2336,7 @@
         <v>67</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>19</v>
@@ -2117,10 +2350,10 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>17</v>
@@ -2137,10 +2370,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>17</v>
@@ -2157,10 +2390,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>17</v>
@@ -2177,10 +2410,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>17</v>
@@ -2227,7 +2460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02C6D364-B355-4419-A681-1738943D0841}">
   <dimension ref="A1:M16"/>
   <sheetViews>
@@ -2359,7 +2592,7 @@
         <v>97</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -2408,12 +2641,12 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[CHG] MAPA DE STAKEHOLDERS
</commit_message>
<xml_diff>
--- a/Mapa de Stakeholders.xlsx
+++ b/Mapa de Stakeholders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e66243f108409f2/Área de Trabalho/Itaú/CICF/Product Manager/excel-backlog-planning-roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="511" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{521ED50A-74A3-41BC-8A4F-A43640FE004E}"/>
+  <xr:revisionPtr revIDLastSave="526" documentId="11_AD4D361C20488DEA4E38A076EC1B5A785BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4EF77FB-6D4C-48C6-A04E-6E0144681827}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entrevistados" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="156">
   <si>
     <t>Grupo</t>
   </si>
@@ -494,55 +494,7 @@
     <t>Liderança de Produto e Operação</t>
   </si>
   <si>
-    <t>Analista/Coord. de Operação</t>
-  </si>
-  <si>
     <t>Foco</t>
-  </si>
-  <si>
-    <t>Execução e entrega de produto</t>
-  </si>
-  <si>
-    <t>Estratégia, performance e decisões macro</t>
-  </si>
-  <si>
-    <t>Frequência</t>
-  </si>
-  <si>
-    <t>Dados exigidos</t>
-  </si>
-  <si>
-    <t>Disponibilidade, saúde, alertas</t>
-  </si>
-  <si>
-    <t>Performance agregada, históricos, OKRs</t>
-  </si>
-  <si>
-    <t>SLA, reincidência, previsão, performance por fornecedor</t>
-  </si>
-  <si>
-    <t>Painel desejado</t>
-  </si>
-  <si>
-    <t>Interativo, com filtros</t>
-  </si>
-  <si>
-    <t>Analítico e consolidado</t>
-  </si>
-  <si>
-    <t>Tático e detalhado com filtros por fornecedor</t>
-  </si>
-  <si>
-    <t>Formato</t>
-  </si>
-  <si>
-    <t>Real time + histórico</t>
-  </si>
-  <si>
-    <t>Dispositivo</t>
-  </si>
-  <si>
-    <t>Eficiência e performance de fornecedores</t>
   </si>
   <si>
     <t>Tomar decisões estratégicas com base em dados de disponibilidade de agência.</t>
@@ -569,13 +521,82 @@
   </si>
   <si>
     <t>Rogerio Vasconcelos Costa</t>
+  </si>
+  <si>
+    <t>Performance e evolução do produto</t>
+  </si>
+  <si>
+    <t>Estratégia e eficiência operacional</t>
+  </si>
+  <si>
+    <t>Eficiência de fornecedores</t>
+  </si>
+  <si>
+    <t>Continuidade do atendimento físico</t>
+  </si>
+  <si>
+    <t>Frequência de uso</t>
+  </si>
+  <si>
+    <t>Formato desejado</t>
+  </si>
+  <si>
+    <t>Real time + Histórico</t>
+  </si>
+  <si>
+    <t>Dispositivo principal</t>
+  </si>
+  <si>
+    <t>Indicadores-chave</t>
+  </si>
+  <si>
+    <t>Indisponibilidade, saúde, reincidência</t>
+  </si>
+  <si>
+    <t>OKRs, capacidade, causa raiz</t>
+  </si>
+  <si>
+    <t>SLA, long tail, reincidência</t>
+  </si>
+  <si>
+    <t>Alertas e painéis com filtros</t>
+  </si>
+  <si>
+    <t>Visão analítica e consolidada</t>
+  </si>
+  <si>
+    <t>Comparação de fornecedores, alertas</t>
+  </si>
+  <si>
+    <t>SLA diferenciado, visões por bairro</t>
+  </si>
+  <si>
+    <t>Tipo de ação esperada</t>
+  </si>
+  <si>
+    <t>Correções táticas e melhorias no produto</t>
+  </si>
+  <si>
+    <t>Priorização estratégica e planejamento</t>
+  </si>
+  <si>
+    <t>Correções com fornecedores</t>
+  </si>
+  <si>
+    <t>Tomada de decisão local imediata</t>
+  </si>
+  <si>
+    <t>Analista e Coordenador de Operação</t>
+  </si>
+  <si>
+    <t>Agências indisponíveis, equipamentos, quantidade de clientes impactados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -594,6 +615,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -765,7 +794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -854,6 +883,21 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -884,19 +928,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -914,42 +946,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1009,6 +1005,42 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1030,89 +1062,89 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F1246330-6313-46DC-940B-D8072DA36581}" name="tbStakeholders" displayName="tbStakeholders" ref="A1:J23" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F1246330-6313-46DC-940B-D8072DA36581}" name="tbStakeholders" displayName="tbStakeholders" ref="A1:J23" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:J23" xr:uid="{F1246330-6313-46DC-940B-D8072DA36581}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{475B94CC-9EDA-43B2-AADB-D9D139409FEE}" name="Nome do Stakeholder" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{C29DFBFA-E5F5-479F-A17D-237E9FA0A2DC}" name="Papel/Função" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{F71A8DF8-2F2A-4196-B9BB-D950577B7A66}" name="Organização/Área" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{AACAD26B-0A16-4396-A845-9C577BED7FA6}" name="Tipo (Interno/Externo)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{61CDD6E8-E23B-4639-82AA-0D92DAE2BC92}" name="Nível de Influência" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{7DF80E76-E50B-4DC0-9A2C-A346F41DEF03}" name="Nível de Interesse" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{5EC43087-AA8B-45BE-8B11-FC2DC98C68ED}" name="Expectativas/Interesses" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{E5AC54B5-3304-4CC7-9F2F-56A8B94187A6}" name="Comunicação Preferencial" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{6B2B5879-1AAB-47D0-8B0F-7CD8C9CAF668}" name="Participação Esperada" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{9C1F95B2-F159-4188-9916-577765EEEE3C}" name="Notas Adicionais" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{475B94CC-9EDA-43B2-AADB-D9D139409FEE}" name="Nome do Stakeholder" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{C29DFBFA-E5F5-479F-A17D-237E9FA0A2DC}" name="Papel/Função" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{F71A8DF8-2F2A-4196-B9BB-D950577B7A66}" name="Organização/Área" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{AACAD26B-0A16-4396-A845-9C577BED7FA6}" name="Tipo (Interno/Externo)" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{61CDD6E8-E23B-4639-82AA-0D92DAE2BC92}" name="Nível de Influência" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{7DF80E76-E50B-4DC0-9A2C-A346F41DEF03}" name="Nível de Interesse" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{5EC43087-AA8B-45BE-8B11-FC2DC98C68ED}" name="Expectativas/Interesses" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{E5AC54B5-3304-4CC7-9F2F-56A8B94187A6}" name="Comunicação Preferencial" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{6B2B5879-1AAB-47D0-8B0F-7CD8C9CAF668}" name="Participação Esperada" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{9C1F95B2-F159-4188-9916-577765EEEE3C}" name="Notas Adicionais" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E6735BAA-6C0B-4784-8A94-1A274CFA1DA1}" name="tbPapelFuncao" displayName="tbPapelFuncao" ref="A1:A16" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E6735BAA-6C0B-4784-8A94-1A274CFA1DA1}" name="tbPapelFuncao" displayName="tbPapelFuncao" ref="A1:A16" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:A16" xr:uid="{E6735BAA-6C0B-4784-8A94-1A274CFA1DA1}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{1A2E27DC-5620-4CDF-92D6-2CDD6C74D104}" name="Papel/Função" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{1A2E27DC-5620-4CDF-92D6-2CDD6C74D104}" name="Papel/Função" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D00769C5-549D-4CF7-8F8B-2829D646AED8}" name="tbOrganizacaoArea" displayName="tbOrganizacaoArea" ref="C1:C10" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D00769C5-549D-4CF7-8F8B-2829D646AED8}" name="tbOrganizacaoArea" displayName="tbOrganizacaoArea" ref="C1:C10" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="C1:C10" xr:uid="{D00769C5-549D-4CF7-8F8B-2829D646AED8}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{FE071EE0-E939-4319-BB24-105D65C970FF}" name="Organização/Área" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{FE071EE0-E939-4319-BB24-105D65C970FF}" name="Organização/Área" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{251A06F2-A6A8-4136-9272-3BF6D8A653F2}" name="tbInternoExterno" displayName="tbInternoExterno" ref="E1:E3" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{251A06F2-A6A8-4136-9272-3BF6D8A653F2}" name="tbInternoExterno" displayName="tbInternoExterno" ref="E1:E3" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="E1:E3" xr:uid="{251A06F2-A6A8-4136-9272-3BF6D8A653F2}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C9AD1377-F7E5-45A7-8C64-F27BDA8675B6}" name="Tipo (Interno/Externo)" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{C9AD1377-F7E5-45A7-8C64-F27BDA8675B6}" name="Tipo (Interno/Externo)" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{82503D68-9D13-4B6B-B2E4-02571E78B1B0}" name="tbNivelInfluencia" displayName="tbNivelInfluencia" ref="G1:G4" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{82503D68-9D13-4B6B-B2E4-02571E78B1B0}" name="tbNivelInfluencia" displayName="tbNivelInfluencia" ref="G1:G4" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="G1:G4" xr:uid="{82503D68-9D13-4B6B-B2E4-02571E78B1B0}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{F733C1CF-DA3C-4EDA-AFCF-989713B1D6C2}" name="Nível de Influência" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{F733C1CF-DA3C-4EDA-AFCF-989713B1D6C2}" name="Nível de Influência" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5D8A4B15-96F6-43FB-8638-03423FA7F873}" name="tbInteresse" displayName="tbInteresse" ref="I1:I4" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5D8A4B15-96F6-43FB-8638-03423FA7F873}" name="tbInteresse" displayName="tbInteresse" ref="I1:I4" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="I1:I4" xr:uid="{5D8A4B15-96F6-43FB-8638-03423FA7F873}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{1ABAA705-B50C-4A41-A7DC-FCA27A201C0E}" name="Nível de Interesse" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{1ABAA705-B50C-4A41-A7DC-FCA27A201C0E}" name="Nível de Interesse" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{82452973-7A68-41C8-8BDF-EAB5474FF63F}" name="tbComunicacao" displayName="tbComunicacao" ref="K1:K4" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{82452973-7A68-41C8-8BDF-EAB5474FF63F}" name="tbComunicacao" displayName="tbComunicacao" ref="K1:K4" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="K1:K4" xr:uid="{82452973-7A68-41C8-8BDF-EAB5474FF63F}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{20E8362D-378B-4BB7-B236-59B94A0DCB12}" name="Comunicação Preferencial" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{20E8362D-378B-4BB7-B236-59B94A0DCB12}" name="Comunicação Preferencial" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{43D33FD8-901B-4929-BBC2-E18075F2DB09}" name="tbParticipacao" displayName="tbParticipacao" ref="M1:M5" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{43D33FD8-901B-4929-BBC2-E18075F2DB09}" name="tbParticipacao" displayName="tbParticipacao" ref="M1:M5" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="M1:M5" xr:uid="{43D33FD8-901B-4929-BBC2-E18075F2DB09}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{F5501E43-A4A4-4E99-B968-CCA1CCE993D3}" name="Participação Esperada" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{F5501E43-A4A4-4E99-B968-CCA1CCE993D3}" name="Participação Esperada" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1474,25 +1506,25 @@
       <c r="D2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="35" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1509,13 +1541,13 @@
       <c r="D3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="31"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="36"/>
     </row>
     <row r="4" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
@@ -1530,30 +1562,30 @@
       <c r="D4" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="H4" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="J4" s="32" t="s">
+      <c r="J4" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="34" t="s">
+      <c r="K4" s="39" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="31" t="s">
         <v>66</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -1565,13 +1597,13 @@
       <c r="D5" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="35"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="40"/>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
@@ -1586,13 +1618,13 @@
       <c r="D6" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="35"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="40"/>
     </row>
     <row r="7" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
@@ -1607,13 +1639,13 @@
       <c r="D7" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="35"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="40"/>
     </row>
     <row r="8" spans="1:11" ht="172.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
@@ -1628,25 +1660,25 @@
       <c r="D8" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="E8" s="41" t="s">
-        <v>143</v>
-      </c>
-      <c r="F8" s="41" t="s">
+      <c r="E8" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="G8" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="H8" s="41" t="s">
+      <c r="H8" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="I8" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="40" t="s">
+      <c r="J8" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="K8" s="40" t="s">
+      <c r="K8" s="33" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1663,13 +1695,13 @@
       <c r="D9" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
     </row>
     <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
@@ -1682,13 +1714,13 @@
         <v>106</v>
       </c>
       <c r="D10" s="27"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
     </row>
     <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
@@ -1703,13 +1735,13 @@
       <c r="D11" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
     </row>
     <row r="12" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
@@ -1722,25 +1754,25 @@
         <v>108</v>
       </c>
       <c r="D12" s="29"/>
-      <c r="E12" s="43" t="s">
-        <v>142</v>
-      </c>
-      <c r="F12" s="43" t="s">
-        <v>144</v>
-      </c>
-      <c r="G12" s="43" t="s">
-        <v>145</v>
-      </c>
-      <c r="H12" s="43" t="s">
-        <v>146</v>
-      </c>
-      <c r="I12" s="43" t="s">
+      <c r="E12" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="H12" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="I12" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="J12" s="43" t="s">
+      <c r="J12" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="K12" s="43" t="s">
+      <c r="K12" s="32" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1755,15 +1787,15 @@
         <v>108</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
+        <v>131</v>
+      </c>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
@@ -1776,32 +1808,18 @@
         <v>109</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
+        <v>132</v>
+      </c>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="G8:G11"/>
-    <mergeCell ref="H8:H11"/>
-    <mergeCell ref="I8:I11"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="E4:E7"/>
     <mergeCell ref="F4:F7"/>
@@ -1816,6 +1834,20 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="G8:G11"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="I12:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1823,48 +1855,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{896AFEEB-F632-4315-844F-C80E2D24D70E}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="29.88671875" style="2" customWidth="1"/>
+    <col min="1" max="5" width="36.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="42" t="s">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="30"/>
+      <c r="B1" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="45" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
-        <v>126</v>
-      </c>
       <c r="B2" s="7" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
-        <v>129</v>
+        <v>135</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="45" t="s">
+        <v>137</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>56</v>
@@ -1875,61 +1909,93 @@
       <c r="D3" s="7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="42" t="s">
-        <v>130</v>
+      <c r="E3" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="45" t="s">
+        <v>138</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="42" t="s">
-        <v>134</v>
+        <v>115</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="45" t="s">
+        <v>140</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>135</v>
+        <v>59</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>136</v>
+        <v>83</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="42" t="s">
-        <v>138</v>
+        <v>59</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="45" t="s">
+        <v>141</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
-        <v>140</v>
+        <v>144</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="45" t="s">
+        <v>49</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>59</v>
+        <v>145</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>83</v>
+        <v>146</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>59</v>
+        <v>147</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>